<commit_message>
added all categories, isAdmin & + group comment progress
</commit_message>
<xml_diff>
--- a/categories.xlsx
+++ b/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gfields/INFO 442/team-e/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brick\Go\src\442GroupsProject\team-e\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE64F1D-FC8A-D74F-AC87-6CB3C6CAD1B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B7BE5C-EFDC-40C6-B360-853023CE0378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{B9F14D3A-FC33-D043-84F3-F6DE5D7296CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B9F14D3A-FC33-D043-84F3-F6DE5D7296CF}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
@@ -34,26 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>DIY</t>
   </si>
   <si>
-    <t>Movies</t>
-  </si>
-  <si>
-    <t>Documentaries</t>
-  </si>
-  <si>
-    <t>Gardening</t>
-  </si>
-  <si>
     <t>Camping</t>
   </si>
   <si>
-    <t>Board Games</t>
-  </si>
-  <si>
     <t>Music</t>
   </si>
   <si>
@@ -63,15 +51,6 @@
     <t>Investing</t>
   </si>
   <si>
-    <t>Budgeting</t>
-  </si>
-  <si>
-    <t>Volunteer</t>
-  </si>
-  <si>
-    <t>Yoga</t>
-  </si>
-  <si>
     <t>Writing</t>
   </si>
   <si>
@@ -102,21 +81,6 @@
     <t>Programming</t>
   </si>
   <si>
-    <t>Calligraphy</t>
-  </si>
-  <si>
-    <t>Photography</t>
-  </si>
-  <si>
-    <t>Drawing</t>
-  </si>
-  <si>
-    <t>Painting</t>
-  </si>
-  <si>
-    <t>Animals</t>
-  </si>
-  <si>
     <t>Cars</t>
   </si>
   <si>
@@ -126,9 +90,6 @@
     <t>Shopping</t>
   </si>
   <si>
-    <t>Baking</t>
-  </si>
-  <si>
     <t>Collecting</t>
   </si>
   <si>
@@ -147,15 +108,9 @@
     <t>Tutoring</t>
   </si>
   <si>
-    <t>Swimming</t>
-  </si>
-  <si>
     <t>Poetry</t>
   </si>
   <si>
-    <t>Crafting</t>
-  </si>
-  <si>
     <t>Internships</t>
   </si>
   <si>
@@ -165,16 +120,55 @@
     <t>Gaming</t>
   </si>
   <si>
-    <t>Television</t>
-  </si>
-  <si>
-    <t>Coding</t>
-  </si>
-  <si>
     <t>Content Creation</t>
   </si>
   <si>
-    <t>Coffee</t>
+    <t>Volunteering</t>
+  </si>
+  <si>
+    <t>Card &amp; Board Games</t>
+  </si>
+  <si>
+    <t>Movies &amp; TV</t>
+  </si>
+  <si>
+    <t>Academics</t>
+  </si>
+  <si>
+    <t>Animals &amp; Pets</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Drawing &amp; Painting</t>
+  </si>
+  <si>
+    <t>Yoga &amp; Mindfulness</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Photography &amp; Video</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Crafts</t>
+  </si>
+  <si>
+    <t>Real Estate</t>
   </si>
 </sst>
 </file>
@@ -533,410 +527,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F8AF27-60BB-DA40-A1AF-912013B7D156}">
-  <dimension ref="A1:A98"/>
+  <dimension ref="A1:A85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="2"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="1"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="1"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>